<commit_message>
🧱 units section to staff & students
</commit_message>
<xml_diff>
--- a/backend/output/magic4.xlsx
+++ b/backend/output/magic4.xlsx
@@ -503,25 +503,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8:00 AM to 10:00 AM</t>
+          <t>8:00 AM to 9:00 AM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MITS4003</t>
+          <t>MITS5507</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Sammy</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -593,25 +593,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8:00 AM to 9:00 AM</t>
+          <t>8:00 AM to 10:00 AM</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MITS5507</t>
+          <t>MITS4003</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Sammy</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -653,25 +653,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9:00 AM to 10:00 AM</t>
+          <t>9:00 AM to 11:00 AM</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MITS4004</t>
+          <t>MITS6001</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Kat</t>
+          <t>Josh</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -683,25 +683,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>9:00 AM to 11:00 AM</t>
+          <t>9:00 AM to 10:00 AM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MITS6001</t>
+          <t>MITS4004</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Josh</t>
+          <t>Kat</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -863,20 +863,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2:00 PM to 3:00 PM</t>
+          <t>2:00 PM to 4:00 PM</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MITS6500</t>
+          <t>MITS5003</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Keno</t>
+          <t>Jay</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -893,20 +893,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2:00 PM to 4:00 PM</t>
+          <t>2:00 PM to 3:00 PM</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MITS5003</t>
+          <t>MITS6500</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Jay</t>
+          <t>Keno</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">

</xml_diff>

<commit_message>
Calendar event display html reads properly
</commit_message>
<xml_diff>
--- a/backend/output/magic4.xlsx
+++ b/backend/output/magic4.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -478,15 +478,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MITS5002</t>
+          <t>MITS5507</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mitch</t>
+          <t>Sammy</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -508,15 +508,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MITS5507</t>
+          <t>MITS5002</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Sammy</t>
+          <t>Mitch</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -563,25 +563,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8:00 AM to 10:00 AM</t>
+          <t>8:00 AM to 9:00 AM</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MITS5501</t>
+          <t>MITS4001</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Lewis</t>
+          <t>Jim</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -598,15 +598,15 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MITS4003</t>
+          <t>MITS5501</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Lewis</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -623,25 +623,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>8:00 AM to 9:00 AM</t>
+          <t>8:00 AM to 10:00 AM</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MITS4001</t>
+          <t>MITS4003</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Jim</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -863,20 +863,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2:00 PM to 4:00 PM</t>
+          <t>2:00 PM to 3:00 PM</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MITS5003</t>
+          <t>MITS6500</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Jay</t>
+          <t>Keno</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -893,20 +893,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2:00 PM to 3:00 PM</t>
+          <t>2:00 PM to 4:00 PM</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MITS6500</t>
+          <t>MITS5003</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Keno</t>
+          <t>Jay</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">

</xml_diff>

<commit_message>
🔽add room button buildings page
</commit_message>
<xml_diff>
--- a/backend/output/magic4.xlsx
+++ b/backend/output/magic4.xlsx
@@ -478,15 +478,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MITS5507</t>
+          <t>MITS4001</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sammy</t>
+          <t>Jim</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -508,15 +508,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MITS5501</t>
+          <t>MITS4003</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lewis</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -538,20 +538,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MITS5002</t>
+          <t>MITS5503</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Mitch</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -568,20 +568,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MITS5503</t>
+          <t>MITS5507</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Sammy</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -593,25 +593,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8:00 AM to 9:00 AM</t>
+          <t>8:00 AM to 10:00 AM</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MITS4001</t>
+          <t>MITS5501</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Jim</t>
+          <t>Lewis</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -623,25 +623,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>8:00 AM to 10:00 AM</t>
+          <t>8:00 AM to 9:00 AM</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MITS4003</t>
+          <t>MITS5002</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Mitch</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -653,25 +653,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9:00 AM to 10:00 AM</t>
+          <t>9:00 AM to 11:00 AM</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MITS4004</t>
+          <t>MITS6001</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Kat</t>
+          <t>Josh</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -683,25 +683,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>9:00 AM to 11:00 AM</t>
+          <t>9:00 AM to 10:00 AM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MITS6001</t>
+          <t>MITS4004</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Josh</t>
+          <t>Kat</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -718,15 +718,15 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MITS5004</t>
+          <t>MITS5502</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Sean</t>
+          <t>Jake</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -748,15 +748,15 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MITS5502</t>
+          <t>MITS5004</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Jake</t>
+          <t>Sean</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -863,20 +863,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2:00 PM to 4:00 PM</t>
+          <t>2:00 PM to 3:00 PM</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MITS5003</t>
+          <t>MITS6500</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Jay</t>
+          <t>Keno</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -893,20 +893,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2:00 PM to 3:00 PM</t>
+          <t>2:00 PM to 4:00 PM</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MITS6500</t>
+          <t>MITS5003</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Keno</t>
+          <t>Jay</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">

</xml_diff>

<commit_message>
added processing for collate_info
</commit_message>
<xml_diff>
--- a/backend/output/magic4.xlsx
+++ b/backend/output/magic4.xlsx
@@ -473,25 +473,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8:00 AM to 9:00 AM</t>
+          <t>8:00 AM to 10:00 AM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MITS5002</t>
+          <t>MITS5501</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mitch</t>
+          <t>Lewis</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -508,20 +508,20 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MITS5507</t>
+          <t>MITS5503</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Sammy</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -538,20 +538,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MITS5503</t>
+          <t>MITS4001</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Jim</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -563,25 +563,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8:00 AM to 10:00 AM</t>
+          <t>8:00 AM to 9:00 AM</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MITS5501</t>
+          <t>MITS5507</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Lewis</t>
+          <t>Sammy</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -628,15 +628,15 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MITS4001</t>
+          <t>MITS5002</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Jim</t>
+          <t>Mitch</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">

</xml_diff>

<commit_message>
added csv for collate info
</commit_message>
<xml_diff>
--- a/backend/output/magic4.xlsx
+++ b/backend/output/magic4.xlsx
@@ -478,15 +478,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MITS5501</t>
+          <t>MITS4003</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Lewis</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -503,20 +503,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8:00 AM to 9:00 AM</t>
+          <t>8:00 AM to 10:00 AM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MITS5503</t>
+          <t>MITS5501</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Lewis</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -538,20 +538,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MITS4001</t>
+          <t>MITS5503</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Jim</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -593,25 +593,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8:00 AM to 10:00 AM</t>
+          <t>8:00 AM to 9:00 AM</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MITS4003</t>
+          <t>MITS4001</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Jim</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -718,15 +718,15 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MITS5004</t>
+          <t>MITS5502</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Sean</t>
+          <t>Jake</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -748,15 +748,15 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MITS5502</t>
+          <t>MITS5004</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Jake</t>
+          <t>Sean</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -863,20 +863,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2:00 PM to 4:00 PM</t>
+          <t>2:00 PM to 3:00 PM</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MITS5003</t>
+          <t>MITS6500</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Jay</t>
+          <t>Keno</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -893,20 +893,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2:00 PM to 3:00 PM</t>
+          <t>2:00 PM to 4:00 PM</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MITS6500</t>
+          <t>MITS5003</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Keno</t>
+          <t>Jay</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">

</xml_diff>

<commit_message>
added fetch to backend when generate is clicekd
</commit_message>
<xml_diff>
--- a/backend/output/magic4.xlsx
+++ b/backend/output/magic4.xlsx
@@ -473,20 +473,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8:00 AM to 10:00 AM</t>
+          <t>8:00 AM to 9:00 AM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MITS4003</t>
+          <t>MITS5503</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -503,25 +503,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8:00 AM to 10:00 AM</t>
+          <t>8:00 AM to 9:00 AM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MITS5501</t>
+          <t>MITS5002</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lewis</t>
+          <t>Mitch</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -533,20 +533,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8:00 AM to 9:00 AM</t>
+          <t>8:00 AM to 10:00 AM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MITS5503</t>
+          <t>MITS4003</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -563,25 +563,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8:00 AM to 9:00 AM</t>
+          <t>8:00 AM to 10:00 AM</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MITS5507</t>
+          <t>MITS5501</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Sammy</t>
+          <t>Lewis</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -628,15 +628,15 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MITS5002</t>
+          <t>MITS5507</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Mitch</t>
+          <t>Sammy</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -653,25 +653,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9:00 AM to 11:00 AM</t>
+          <t>9:00 AM to 10:00 AM</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MITS6001</t>
+          <t>MITS4004</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Josh</t>
+          <t>Kat</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -683,25 +683,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>9:00 AM to 10:00 AM</t>
+          <t>9:00 AM to 11:00 AM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MITS4004</t>
+          <t>MITS6001</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Kat</t>
+          <t>Josh</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -718,15 +718,15 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MITS5502</t>
+          <t>MITS5004</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Jake</t>
+          <t>Sean</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -748,15 +748,15 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MITS5004</t>
+          <t>MITS5502</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Sean</t>
+          <t>Jake</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -863,20 +863,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2:00 PM to 3:00 PM</t>
+          <t>2:00 PM to 4:00 PM</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MITS6500</t>
+          <t>MITS5003</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Keno</t>
+          <t>Jay</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -893,20 +893,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2:00 PM to 4:00 PM</t>
+          <t>2:00 PM to 3:00 PM</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MITS5003</t>
+          <t>MITS6500</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Jay</t>
+          <t>Keno</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">

</xml_diff>

<commit_message>
Default color and form changes
</commit_message>
<xml_diff>
--- a/backend/output/magic4.xlsx
+++ b/backend/output/magic4.xlsx
@@ -478,15 +478,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MITS5507</t>
+          <t>MITS4001</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sammy</t>
+          <t>Jim</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -508,15 +508,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MITS5002</t>
+          <t>MITS5507</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Mitch</t>
+          <t>Sammy</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -568,15 +568,15 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MITS4001</t>
+          <t>MITS5002</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Jim</t>
+          <t>Mitch</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -653,25 +653,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9:00 AM to 11:00 AM</t>
+          <t>9:00 AM to 10:00 AM</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MITS6001</t>
+          <t>MITS4004</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Josh</t>
+          <t>Kat</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>F2F</t>
+          <t>Online</t>
         </is>
       </c>
     </row>
@@ -683,25 +683,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>9:00 AM to 10:00 AM</t>
+          <t>9:00 AM to 11:00 AM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MITS4004</t>
+          <t>MITS6001</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Kat</t>
+          <t>Josh</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>F2F</t>
         </is>
       </c>
     </row>
@@ -718,15 +718,15 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MITS5004</t>
+          <t>MITS5502</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Sean</t>
+          <t>Jake</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -748,15 +748,15 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MITS5502</t>
+          <t>MITS5004</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Jake</t>
+          <t>Sean</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">

</xml_diff>